<commit_message>
Clarifying column headers and annotations in code
</commit_message>
<xml_diff>
--- a/Data/20241203_CCSLysoTrackerRaw.xlsx
+++ b/Data/20241203_CCSLysoTrackerRaw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/RawData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{E708E5CC-0F2A-5742-A435-85B68EEDC36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{C7262052-C30E-8F40-9996-C31681BA4CFB}"/>
+    <workbookView xWindow="35700" yWindow="1300" windowWidth="27240" windowHeight="16440" xr2:uid="{C7262052-C30E-8F40-9996-C31681BA4CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
   <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>